<commit_message>
Version of board with small 5.1x5.1 smd tactile buttons
</commit_message>
<xml_diff>
--- a/MFD/Project Outputs for Mfd3/Bill of Materials-Mfd3.xlsx
+++ b/MFD/Project Outputs for Mfd3/Bill of Materials-Mfd3.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="84">
   <si>
     <t>Comment</t>
   </si>
@@ -90,13 +90,13 @@
     <t>C16133</t>
   </si>
   <si>
-    <t>IDC 2X4 2.54</t>
-  </si>
-  <si>
-    <t>IDC socket, 4-Pin, Dual row, 2.54 mm</t>
-  </si>
-  <si>
-    <t>P1</t>
+    <t>LED 0603</t>
+  </si>
+  <si>
+    <t>LED1, LED2, LED3, LED4, LED5, LED6, LED7, LED8, LED9, LED10, LED11, LED12, LED13, LED14, LED15, LED16, LED17, LED18, LED19, LED20, LED21, LED22, LED23, LED24, LED25, LED26, LED27, LED28, LED29, LED30, LED31, LED32, LED33, LED34</t>
+  </si>
+  <si>
+    <t>C72043</t>
   </si>
   <si>
     <t>PLD 1X4H</t>
@@ -126,12 +126,6 @@
     <t>P4</t>
   </si>
   <si>
-    <t>USB-B</t>
-  </si>
-  <si>
-    <t>P5</t>
-  </si>
-  <si>
     <t>10K</t>
   </si>
   <si>
@@ -189,13 +183,16 @@
     <t>C4310</t>
   </si>
   <si>
-    <t>TS-H003</t>
-  </si>
-  <si>
-    <t>AKEYS TS-H003</t>
+    <t>TACT SWITCH 5.2mm</t>
+  </si>
+  <si>
+    <t>Push button 5.2 mm</t>
   </si>
   <si>
     <t>SW1, SW2, SW3, SW4, SW5, SW6, SW7, SW8, SW9, SW10, SW11, SW12, SW13, SW14, SW15, SW16, SW17, SW18, SW19, SW20, SW21, SW22, SW23, SW24, SW25, SW26, SW27, SW28, SW29, SW30, SW31, SW32, SW33, SW34</t>
+  </si>
+  <si>
+    <t>C412369</t>
   </si>
   <si>
     <t>WS-TASV SMD Tact Switch 6.0X3.5 mm</t>
@@ -643,7 +640,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -753,23 +750,25 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="30">
+    <row r="6" spans="1:6" ht="180">
       <c r="A6" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>25</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E6" s="4">
-        <v>1</v>
-      </c>
-      <c r="F6" s="4"/>
+        <v>34</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="7" spans="1:6" ht="30">
       <c r="A7" s="3" t="s">
@@ -825,264 +824,248 @@
       </c>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" ht="135">
       <c r="A10" s="3" t="s">
         <v>35</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E10" s="4">
-        <v>1</v>
-      </c>
-      <c r="F10" s="4"/>
+        <v>37</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="11" spans="1:6" ht="135">
       <c r="A11" s="3" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>40</v>
-      </c>
       <c r="E11" s="4">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="135">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>40</v>
-      </c>
       <c r="E12" s="4">
-        <v>34</v>
+        <v>2</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B13" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>40</v>
       </c>
       <c r="E13" s="4">
         <v>2</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="E14" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="180">
       <c r="A15" s="3" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>54</v>
       </c>
       <c r="E15" s="4">
+        <v>34</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="30">
+      <c r="A16" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E16" s="4">
         <v>1</v>
       </c>
-      <c r="F15" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="180">
-      <c r="A16" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E16" s="4">
-        <v>34</v>
-      </c>
       <c r="F16" s="4"/>
     </row>
-    <row r="17" spans="1:6" ht="30">
+    <row r="17" spans="1:6" ht="45">
       <c r="A17" s="3" t="s">
-        <v>33</v>
+        <v>61</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="E17" s="4">
+        <v>4</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="75">
+      <c r="A18" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E18" s="4">
         <v>1</v>
       </c>
-      <c r="F17" s="4"/>
-    </row>
-    <row r="18" spans="1:6" ht="45">
-      <c r="A18" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E18" s="4">
-        <v>4</v>
-      </c>
       <c r="F18" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="75">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="30">
       <c r="A19" s="3" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="E19" s="4">
         <v>1</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="30">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20" s="3" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>73</v>
+        <v>36</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>75</v>
+        <v>38</v>
       </c>
       <c r="E20" s="4">
+        <v>2</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="60">
+      <c r="A21" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E21" s="4">
         <v>1</v>
       </c>
-      <c r="F20" s="3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="E21" s="4">
-        <v>2</v>
-      </c>
       <c r="F21" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="60">
-      <c r="A22" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="D22" s="3" t="s">
         <v>83</v>
-      </c>
-      <c r="E22" s="4">
-        <v>1</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>84</v>
       </c>
     </row>
   </sheetData>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.30555555555555558" right="0.30555555555555558" top="0.30555555555555558" bottom="0.30555555555555558" header="0" footer="0"/>
-  <pageSetup paperSize="9" scale="56" orientation="landscape" blackAndWhite="1" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="49" orientation="landscape" blackAndWhite="1" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Replaced TS-H003 with TM-001-M-04 button
</commit_message>
<xml_diff>
--- a/MFD/Project Outputs for Mfd3/Bill of Materials-Mfd3.xlsx
+++ b/MFD/Project Outputs for Mfd3/Bill of Materials-Mfd3.xlsx
@@ -8,8 +8,6 @@
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-Mfd3" sheetId="1" r:id="rId1"/>
-    <sheet name="Лист2" sheetId="2" r:id="rId2"/>
-    <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Bill of Materials-Mfd3'!$1:$1</definedName>
@@ -19,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="86">
   <si>
     <t>Comment</t>
   </si>
@@ -36,9 +34,6 @@
     <t>Quantity</t>
   </si>
   <si>
-    <t>LCSC Part #</t>
-  </si>
-  <si>
     <t>0.1 uF</t>
   </si>
   <si>
@@ -198,6 +193,9 @@
     <t>SW1, SW2, SW3, SW4, SW5, SW6, SW7, SW8, SW9, SW10, SW11, SW12, SW13, SW14, SW15, SW16, SW17, SW18, SW19, SW20, SW21, SW22, SW23, SW24, SW25, SW26, SW27, SW28, SW29, SW30, SW31, SW32, SW33, SW34</t>
   </si>
   <si>
+    <t>C2884874</t>
+  </si>
+  <si>
     <t>WS-TASV SMD Tact Switch 6.0X3.5 mm</t>
   </si>
   <si>
@@ -274,6 +272,9 @@
   </si>
   <si>
     <t>C115962</t>
+  </si>
+  <si>
+    <t>JLCPCB Part #</t>
   </si>
 </sst>
 </file>
@@ -331,7 +332,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -341,9 +342,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -645,7 +643,9 @@
   </sheetPr>
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -670,101 +670,101 @@
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>5</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="45">
       <c r="A2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>9</v>
       </c>
       <c r="E2" s="4">
         <v>10</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>12</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>13</v>
       </c>
       <c r="E3" s="4">
         <v>2</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>16</v>
-      </c>
       <c r="D4" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E4" s="4">
         <v>1</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="30">
       <c r="A5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="C5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="D5" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>21</v>
       </c>
       <c r="E5" s="4">
         <v>2</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="30">
       <c r="A6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="C6" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>25</v>
-      </c>
       <c r="D6" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E6" s="4">
         <v>1</v>
@@ -773,16 +773,16 @@
     </row>
     <row r="7" spans="1:6" ht="30">
       <c r="A7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="C7" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>28</v>
-      </c>
       <c r="D7" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E7" s="4">
         <v>2</v>
@@ -791,16 +791,16 @@
     </row>
     <row r="8" spans="1:6" ht="30">
       <c r="A8" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="C8" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>31</v>
-      </c>
       <c r="D8" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E8" s="4">
         <v>1</v>
@@ -809,16 +809,16 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="C9" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>34</v>
-      </c>
       <c r="D9" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E9" s="4">
         <v>1</v>
@@ -827,16 +827,16 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>36</v>
-      </c>
       <c r="D10" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E10" s="4">
         <v>1</v>
@@ -845,125 +845,127 @@
     </row>
     <row r="11" spans="1:6" ht="135">
       <c r="A11" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="C11" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="D11" s="3" t="s">
         <v>39</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>40</v>
       </c>
       <c r="E11" s="4">
         <v>37</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="135">
       <c r="A12" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>43</v>
-      </c>
       <c r="D12" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E12" s="4">
         <v>34</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>46</v>
-      </c>
       <c r="D13" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E13" s="4">
         <v>2</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>49</v>
-      </c>
       <c r="D14" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E14" s="4">
         <v>2</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="C15" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="D15" s="3" t="s">
         <v>53</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>54</v>
       </c>
       <c r="E15" s="4">
         <v>1</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="180">
       <c r="A16" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="C16" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>58</v>
-      </c>
       <c r="D16" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E16" s="4">
         <v>34</v>
       </c>
-      <c r="F16" s="4"/>
+      <c r="F16" s="3" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="17" spans="1:6" ht="30">
       <c r="A17" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>59</v>
@@ -1044,13 +1046,13 @@
         <v>77</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>78</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E21" s="4">
         <v>2</v>
@@ -1084,46 +1086,4 @@
   <pageMargins left="0.30555555555555558" right="0.30555555555555558" top="0.30555555555555558" bottom="0.30555555555555558" header="0" footer="0"/>
   <pageSetup paperSize="9" scale="56" orientation="landscape" blackAndWhite="1" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" s="5"/>
-    </row>
-  </sheetData>
-  <printOptions horizontalCentered="1" verticalCentered="1"/>
-  <pageMargins left="0.30555555555555558" right="0.30555555555555558" top="0.30555555555555558" bottom="0.30555555555555558" header="0" footer="0"/>
-  <pageSetup paperSize="9" orientation="landscape" blackAndWhite="1" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" s="5"/>
-    </row>
-  </sheetData>
-  <printOptions horizontalCentered="1" verticalCentered="1"/>
-  <pageMargins left="0.30555555555555558" right="0.30555555555555558" top="0.30555555555555558" bottom="0.30555555555555558" header="0" footer="0"/>
-  <pageSetup paperSize="9" orientation="landscape" blackAndWhite="1" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>